<commit_message>
Se actualizan entradas y salidas y parametros.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas Y SALIDAS ACIDWASH.xlsX
+++ b/Diagramas/entradas Y SALIDAS ACIDWASH.xlsX
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ENTRADAS</t>
   </si>
@@ -118,13 +118,22 @@
   </si>
   <si>
     <t>PARO</t>
+  </si>
+  <si>
+    <t>ACID WASH</t>
+  </si>
+  <si>
+    <t>PELIGRO</t>
+  </si>
+  <si>
+    <t>VOLTAJE DE CONTROL A 220VOLTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +151,13 @@
     <font>
       <sz val="28"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -202,11 +218,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,16 +271,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -319,6 +387,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -353,6 +422,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -528,206 +598,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" customWidth="1"/>
     <col min="5" max="5" width="97.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
     <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="E3" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="E5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A12:C12"/>
+  <mergeCells count="5">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A1:E3"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="77" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="36">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="36">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="36">
+    <row r="4" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="2:2" ht="36">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="36">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="36">
+    <row r="7" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="2:2" ht="36">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="36">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="2:2" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -738,12 +855,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>